<commit_message>
Vorlage von Mathias nur leicht angepasst, damit auch die gefordete Summe über die Gesamtdauer angezeigt wird
git-svn-id: https://gforge.zih.tu-dresden.de/svn/c0h0@39 9a665d2c-7092-0410-b790-bb0f4d5e5a57
</commit_message>
<xml_diff>
--- a/zeitabrechnung/Vorlage_Zeitabrechnung.xlsx
+++ b/zeitabrechnung/Vorlage_Zeitabrechnung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="14115" windowHeight="7995"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Datum</t>
   </si>
@@ -25,13 +25,34 @@
   </si>
   <si>
     <t>Bearbeitungszeit</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Vorname:</t>
+  </si>
+  <si>
+    <t>Projekt:</t>
+  </si>
+  <si>
+    <t>C0/H0 Transformation</t>
+  </si>
+  <si>
+    <t>gesamte Arbeitsdauer:</t>
+  </si>
+  <si>
+    <t>Zeitprotokoll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd:hh:mm"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,16 +60,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -99,11 +154,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -114,9 +217,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
+    <cellStyle name="Berechnung" xfId="2" builtinId="22"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Zelle überprüfen" xfId="3" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -129,7 +243,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -203,7 +317,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -238,7 +351,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -414,21 +526,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="6"/>
     <col min="2" max="2" width="54.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
+    <col min="5" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -438,37 +551,69 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="5"/>
       <c r="B2" s="8"/>
       <c r="C2" s="2"/>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="E3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="13">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>